<commit_message>
Print MATLAB-style type information
</commit_message>
<xml_diff>
--- a/test/xlsx/h5showList.xlsx
+++ b/test/xlsx/h5showList.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Globals" sheetId="1" r:id="rId1"/>
     <sheet name="h5showList" sheetId="2" r:id="rId2"/>
     <sheet name="h5showList1" sheetId="3" r:id="rId3"/>
     <sheet name="h5showList2" sheetId="4" r:id="rId4"/>
+    <sheet name="h5showList3" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="258">
   <si>
     <t>Home</t>
   </si>
@@ -391,18 +392,12 @@
     <t>StructMetadata.0</t>
   </si>
   <si>
-    <t>|S32000</t>
-  </si>
-  <si>
     <t>()</t>
   </si>
   <si>
     <t>coremetadata.0</t>
   </si>
   <si>
-    <t>|S65535</t>
-  </si>
-  <si>
     <t>/g1</t>
   </si>
   <si>
@@ -415,9 +410,6 @@
     <t>dset1.1.1</t>
   </si>
   <si>
-    <t>&gt;i4</t>
-  </si>
-  <si>
     <t>(10, 10)</t>
   </si>
   <si>
@@ -439,9 +431,6 @@
     <t>dset2.1</t>
   </si>
   <si>
-    <t>&gt;f4</t>
-  </si>
-  <si>
     <t>(10,)</t>
   </si>
   <si>
@@ -752,6 +741,57 @@
   </si>
   <si>
     <t>C:\Users\Gerd\git\PyHexad\</t>
+  </si>
+  <si>
+    <t>string32000</t>
+  </si>
+  <si>
+    <t>string65535</t>
+  </si>
+  <si>
+    <t>Tick data</t>
+  </si>
+  <si>
+    <t>TABLE</t>
+  </si>
+  <si>
+    <t>21-09-2011</t>
+  </si>
+  <si>
+    <t>Time,string16,Bid,float32,Ask,float32</t>
+  </si>
+  <si>
+    <t>(21684,)</t>
+  </si>
+  <si>
+    <t>18-09-2011</t>
+  </si>
+  <si>
+    <t>(2470,)</t>
+  </si>
+  <si>
+    <t>19-09-2011</t>
+  </si>
+  <si>
+    <t>(14711,)</t>
+  </si>
+  <si>
+    <t>22-09-2011</t>
+  </si>
+  <si>
+    <t>(23536,)</t>
+  </si>
+  <si>
+    <t>20-09-2011</t>
+  </si>
+  <si>
+    <t>(16954,)</t>
+  </si>
+  <si>
+    <t>23-09-2011</t>
+  </si>
+  <si>
+    <t>(17969,)</t>
   </si>
 </sst>
 </file>
@@ -1123,10 +1163,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1140,7 +1180,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1168,6 +1208,15 @@
       <c r="B4" t="str">
         <f>CONCATENATE($B1,"testfiles\group100.h5")</f>
         <v>C:\Users\Gerd\git\PyHexad\testfiles\group100.h5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B5" t="str">
+        <f>CONCATENATE($B1,"testfiles\cadchftickdata.h5")</f>
+        <v>C:\Users\Gerd\git\PyHexad\testfiles\cadchftickdata.h5</v>
       </c>
     </row>
   </sheetData>
@@ -3469,13 +3518,13 @@
         <v>0</v>
       </c>
       <c r="F102" t="s">
+        <v>241</v>
+      </c>
+      <c r="G102">
+        <v>0</v>
+      </c>
+      <c r="H102" t="s">
         <v>124</v>
-      </c>
-      <c r="G102">
-        <v>0</v>
-      </c>
-      <c r="H102" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
@@ -3486,19 +3535,19 @@
         <v>21</v>
       </c>
       <c r="C103" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D103">
         <v>0</v>
       </c>
       <c r="F103" t="s">
-        <v>127</v>
+        <v>242</v>
       </c>
       <c r="G103">
         <v>0</v>
       </c>
       <c r="H103" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -3585,7 +3634,7 @@
         <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -3602,7 +3651,7 @@
         <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -3616,22 +3665,22 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D6">
         <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>132</v>
+        <v>106</v>
       </c>
       <c r="G6">
         <v>2</v>
       </c>
       <c r="H6" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -3639,22 +3688,22 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C7" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
       <c r="F7" t="s">
+        <v>106</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7" t="s">
         <v>132</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-      <c r="H7" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -3665,7 +3714,7 @@
         <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -3682,7 +3731,7 @@
         <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -3699,7 +3748,7 @@
         <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -3713,22 +3762,22 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C11" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D11">
         <v>0</v>
       </c>
       <c r="F11" t="s">
-        <v>140</v>
+        <v>26</v>
       </c>
       <c r="G11">
         <v>1</v>
       </c>
       <c r="H11" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -3736,22 +3785,22 @@
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C12" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D12">
         <v>0</v>
       </c>
       <c r="F12" t="s">
-        <v>140</v>
+        <v>26</v>
       </c>
       <c r="G12">
         <v>2</v>
       </c>
       <c r="H12" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -3763,9 +3812,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I103"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3837,7 +3884,7 @@
         <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -3854,7 +3901,7 @@
         <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -3871,7 +3918,7 @@
         <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -3888,7 +3935,7 @@
         <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -3905,7 +3952,7 @@
         <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -3922,7 +3969,7 @@
         <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -3939,7 +3986,7 @@
         <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -3956,7 +4003,7 @@
         <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -3973,7 +4020,7 @@
         <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -3990,7 +4037,7 @@
         <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -4007,7 +4054,7 @@
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -4024,7 +4071,7 @@
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -4041,7 +4088,7 @@
         <v>13</v>
       </c>
       <c r="C16" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -4058,7 +4105,7 @@
         <v>13</v>
       </c>
       <c r="C17" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -4075,7 +4122,7 @@
         <v>13</v>
       </c>
       <c r="C18" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -4092,7 +4139,7 @@
         <v>13</v>
       </c>
       <c r="C19" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -4109,7 +4156,7 @@
         <v>13</v>
       </c>
       <c r="C20" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -4126,7 +4173,7 @@
         <v>13</v>
       </c>
       <c r="C21" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -4143,7 +4190,7 @@
         <v>13</v>
       </c>
       <c r="C22" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -4160,7 +4207,7 @@
         <v>13</v>
       </c>
       <c r="C23" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -4177,7 +4224,7 @@
         <v>13</v>
       </c>
       <c r="C24" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="D24">
         <v>0</v>
@@ -4194,7 +4241,7 @@
         <v>13</v>
       </c>
       <c r="C25" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -4211,7 +4258,7 @@
         <v>13</v>
       </c>
       <c r="C26" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="D26">
         <v>0</v>
@@ -4228,7 +4275,7 @@
         <v>13</v>
       </c>
       <c r="C27" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="D27">
         <v>0</v>
@@ -4245,7 +4292,7 @@
         <v>13</v>
       </c>
       <c r="C28" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D28">
         <v>0</v>
@@ -4262,7 +4309,7 @@
         <v>13</v>
       </c>
       <c r="C29" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="D29">
         <v>0</v>
@@ -4279,7 +4326,7 @@
         <v>13</v>
       </c>
       <c r="C30" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D30">
         <v>0</v>
@@ -4296,7 +4343,7 @@
         <v>13</v>
       </c>
       <c r="C31" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D31">
         <v>0</v>
@@ -4313,7 +4360,7 @@
         <v>13</v>
       </c>
       <c r="C32" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D32">
         <v>0</v>
@@ -4330,7 +4377,7 @@
         <v>13</v>
       </c>
       <c r="C33" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="D33">
         <v>0</v>
@@ -4347,7 +4394,7 @@
         <v>13</v>
       </c>
       <c r="C34" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D34">
         <v>0</v>
@@ -4364,7 +4411,7 @@
         <v>13</v>
       </c>
       <c r="C35" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D35">
         <v>0</v>
@@ -4381,7 +4428,7 @@
         <v>13</v>
       </c>
       <c r="C36" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D36">
         <v>0</v>
@@ -4398,7 +4445,7 @@
         <v>13</v>
       </c>
       <c r="C37" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="D37">
         <v>0</v>
@@ -4415,7 +4462,7 @@
         <v>13</v>
       </c>
       <c r="C38" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="D38">
         <v>0</v>
@@ -4432,7 +4479,7 @@
         <v>13</v>
       </c>
       <c r="C39" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="D39">
         <v>0</v>
@@ -4449,7 +4496,7 @@
         <v>13</v>
       </c>
       <c r="C40" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D40">
         <v>0</v>
@@ -4466,7 +4513,7 @@
         <v>13</v>
       </c>
       <c r="C41" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="D41">
         <v>0</v>
@@ -4483,7 +4530,7 @@
         <v>13</v>
       </c>
       <c r="C42" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="D42">
         <v>0</v>
@@ -4500,7 +4547,7 @@
         <v>13</v>
       </c>
       <c r="C43" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="D43">
         <v>0</v>
@@ -4517,7 +4564,7 @@
         <v>13</v>
       </c>
       <c r="C44" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D44">
         <v>0</v>
@@ -4534,7 +4581,7 @@
         <v>13</v>
       </c>
       <c r="C45" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D45">
         <v>0</v>
@@ -4551,7 +4598,7 @@
         <v>13</v>
       </c>
       <c r="C46" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="D46">
         <v>0</v>
@@ -4568,7 +4615,7 @@
         <v>13</v>
       </c>
       <c r="C47" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="D47">
         <v>0</v>
@@ -4585,7 +4632,7 @@
         <v>13</v>
       </c>
       <c r="C48" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="D48">
         <v>0</v>
@@ -4602,7 +4649,7 @@
         <v>13</v>
       </c>
       <c r="C49" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="D49">
         <v>0</v>
@@ -4619,7 +4666,7 @@
         <v>13</v>
       </c>
       <c r="C50" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="D50">
         <v>0</v>
@@ -4636,7 +4683,7 @@
         <v>13</v>
       </c>
       <c r="C51" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="D51">
         <v>0</v>
@@ -4653,7 +4700,7 @@
         <v>13</v>
       </c>
       <c r="C52" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D52">
         <v>0</v>
@@ -4670,7 +4717,7 @@
         <v>13</v>
       </c>
       <c r="C53" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="D53">
         <v>0</v>
@@ -4687,7 +4734,7 @@
         <v>13</v>
       </c>
       <c r="C54" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="D54">
         <v>0</v>
@@ -4704,7 +4751,7 @@
         <v>13</v>
       </c>
       <c r="C55" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="D55">
         <v>0</v>
@@ -4721,7 +4768,7 @@
         <v>13</v>
       </c>
       <c r="C56" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="D56">
         <v>0</v>
@@ -4738,7 +4785,7 @@
         <v>13</v>
       </c>
       <c r="C57" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="D57">
         <v>0</v>
@@ -4755,7 +4802,7 @@
         <v>13</v>
       </c>
       <c r="C58" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="D58">
         <v>0</v>
@@ -4772,7 +4819,7 @@
         <v>13</v>
       </c>
       <c r="C59" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="D59">
         <v>0</v>
@@ -4789,7 +4836,7 @@
         <v>13</v>
       </c>
       <c r="C60" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="D60">
         <v>0</v>
@@ -4806,7 +4853,7 @@
         <v>13</v>
       </c>
       <c r="C61" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="D61">
         <v>0</v>
@@ -4823,7 +4870,7 @@
         <v>13</v>
       </c>
       <c r="C62" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="D62">
         <v>0</v>
@@ -4840,7 +4887,7 @@
         <v>13</v>
       </c>
       <c r="C63" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="D63">
         <v>0</v>
@@ -4857,7 +4904,7 @@
         <v>13</v>
       </c>
       <c r="C64" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="D64">
         <v>0</v>
@@ -4874,7 +4921,7 @@
         <v>13</v>
       </c>
       <c r="C65" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D65">
         <v>0</v>
@@ -4891,7 +4938,7 @@
         <v>13</v>
       </c>
       <c r="C66" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="D66">
         <v>0</v>
@@ -4908,7 +4955,7 @@
         <v>13</v>
       </c>
       <c r="C67" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="D67">
         <v>0</v>
@@ -4925,7 +4972,7 @@
         <v>13</v>
       </c>
       <c r="C68" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D68">
         <v>0</v>
@@ -4942,7 +4989,7 @@
         <v>13</v>
       </c>
       <c r="C69" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="D69">
         <v>0</v>
@@ -4959,7 +5006,7 @@
         <v>13</v>
       </c>
       <c r="C70" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="D70">
         <v>0</v>
@@ -4976,7 +5023,7 @@
         <v>13</v>
       </c>
       <c r="C71" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D71">
         <v>0</v>
@@ -4993,7 +5040,7 @@
         <v>13</v>
       </c>
       <c r="C72" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="D72">
         <v>0</v>
@@ -5010,7 +5057,7 @@
         <v>13</v>
       </c>
       <c r="C73" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="D73">
         <v>0</v>
@@ -5027,7 +5074,7 @@
         <v>13</v>
       </c>
       <c r="C74" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="D74">
         <v>0</v>
@@ -5044,7 +5091,7 @@
         <v>13</v>
       </c>
       <c r="C75" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="D75">
         <v>0</v>
@@ -5061,7 +5108,7 @@
         <v>13</v>
       </c>
       <c r="C76" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="D76">
         <v>0</v>
@@ -5078,7 +5125,7 @@
         <v>13</v>
       </c>
       <c r="C77" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="D77">
         <v>0</v>
@@ -5095,7 +5142,7 @@
         <v>13</v>
       </c>
       <c r="C78" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="D78">
         <v>0</v>
@@ -5112,7 +5159,7 @@
         <v>13</v>
       </c>
       <c r="C79" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="D79">
         <v>0</v>
@@ -5129,7 +5176,7 @@
         <v>13</v>
       </c>
       <c r="C80" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="D80">
         <v>0</v>
@@ -5146,7 +5193,7 @@
         <v>13</v>
       </c>
       <c r="C81" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="D81">
         <v>0</v>
@@ -5163,7 +5210,7 @@
         <v>13</v>
       </c>
       <c r="C82" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="D82">
         <v>0</v>
@@ -5180,7 +5227,7 @@
         <v>13</v>
       </c>
       <c r="C83" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D83">
         <v>0</v>
@@ -5197,7 +5244,7 @@
         <v>13</v>
       </c>
       <c r="C84" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="D84">
         <v>0</v>
@@ -5214,7 +5261,7 @@
         <v>13</v>
       </c>
       <c r="C85" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="D85">
         <v>0</v>
@@ -5231,7 +5278,7 @@
         <v>13</v>
       </c>
       <c r="C86" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="D86">
         <v>0</v>
@@ -5248,7 +5295,7 @@
         <v>13</v>
       </c>
       <c r="C87" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="D87">
         <v>0</v>
@@ -5265,7 +5312,7 @@
         <v>13</v>
       </c>
       <c r="C88" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="D88">
         <v>0</v>
@@ -5282,7 +5329,7 @@
         <v>13</v>
       </c>
       <c r="C89" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="D89">
         <v>0</v>
@@ -5299,7 +5346,7 @@
         <v>13</v>
       </c>
       <c r="C90" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="D90">
         <v>0</v>
@@ -5316,7 +5363,7 @@
         <v>13</v>
       </c>
       <c r="C91" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="D91">
         <v>0</v>
@@ -5333,7 +5380,7 @@
         <v>13</v>
       </c>
       <c r="C92" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="D92">
         <v>0</v>
@@ -5350,7 +5397,7 @@
         <v>13</v>
       </c>
       <c r="C93" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="D93">
         <v>0</v>
@@ -5367,7 +5414,7 @@
         <v>13</v>
       </c>
       <c r="C94" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="D94">
         <v>0</v>
@@ -5384,7 +5431,7 @@
         <v>13</v>
       </c>
       <c r="C95" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="D95">
         <v>0</v>
@@ -5401,7 +5448,7 @@
         <v>13</v>
       </c>
       <c r="C96" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="D96">
         <v>0</v>
@@ -5418,7 +5465,7 @@
         <v>13</v>
       </c>
       <c r="C97" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="D97">
         <v>0</v>
@@ -5435,7 +5482,7 @@
         <v>13</v>
       </c>
       <c r="C98" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D98">
         <v>0</v>
@@ -5452,7 +5499,7 @@
         <v>13</v>
       </c>
       <c r="C99" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="D99">
         <v>0</v>
@@ -5469,7 +5516,7 @@
         <v>13</v>
       </c>
       <c r="C100" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="D100">
         <v>0</v>
@@ -5486,7 +5533,7 @@
         <v>13</v>
       </c>
       <c r="C101" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D101">
         <v>0</v>
@@ -5503,7 +5550,7 @@
         <v>13</v>
       </c>
       <c r="C102" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D102">
         <v>0</v>
@@ -5520,13 +5567,219 @@
         <v>13</v>
       </c>
       <c r="C103" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="D103">
         <v>0</v>
       </c>
       <c r="E103">
         <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="35.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="str">
+        <f>_xll.h5showList(Globals!$B5)</f>
+        <v>C:\Users\Gerd\git\PyHexad\testfiles\cadchftickdata.h5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>244</v>
+      </c>
+      <c r="C4" t="s">
+        <v>245</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>246</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>244</v>
+      </c>
+      <c r="C5" t="s">
+        <v>248</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="F5" t="s">
+        <v>246</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>244</v>
+      </c>
+      <c r="C6" t="s">
+        <v>250</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="F6" t="s">
+        <v>246</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C7" t="s">
+        <v>252</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="F7" t="s">
+        <v>246</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>244</v>
+      </c>
+      <c r="C8" t="s">
+        <v>254</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="F8" t="s">
+        <v>246</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>244</v>
+      </c>
+      <c r="C9" t="s">
+        <v>256</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="F9" t="s">
+        <v>246</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9" t="s">
+        <v>257</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Print dataset dimensions in Excel array notation.
Version bump to 0.1.4
</commit_message>
<xml_diff>
--- a/test/xlsx/h5showList.xlsx
+++ b/test/xlsx/h5showList.xlsx
@@ -92,9 +92,6 @@
     <t>int8</t>
   </si>
   <si>
-    <t>(5554, 145)</t>
-  </si>
-  <si>
     <t>10.8MicronExtinction</t>
   </si>
   <si>
@@ -104,9 +101,6 @@
     <t>10.8MicronExtinctionNormChiSq</t>
   </si>
   <si>
-    <t>(5554,)</t>
-  </si>
-  <si>
     <t>10.8MicronExtinctionPrecision</t>
   </si>
   <si>
@@ -224,9 +218,6 @@
     <t>CloudTopPressure</t>
   </si>
   <si>
-    <t>(5554, 1)</t>
-  </si>
-  <si>
     <t>H2O</t>
   </si>
   <si>
@@ -332,9 +323,6 @@
     <t>Pressure</t>
   </si>
   <si>
-    <t>(145,)</t>
-  </si>
-  <si>
     <t>ProfileID</t>
   </si>
   <si>
@@ -392,9 +380,6 @@
     <t>StructMetadata.0</t>
   </si>
   <si>
-    <t>()</t>
-  </si>
-  <si>
     <t>coremetadata.0</t>
   </si>
   <si>
@@ -410,15 +395,9 @@
     <t>dset1.1.1</t>
   </si>
   <si>
-    <t>(10, 10)</t>
-  </si>
-  <si>
     <t>dset1.1.2</t>
   </si>
   <si>
-    <t>(20,)</t>
-  </si>
-  <si>
     <t>/g1/g1.2</t>
   </si>
   <si>
@@ -431,15 +410,9 @@
     <t>dset2.1</t>
   </si>
   <si>
-    <t>(10,)</t>
-  </si>
-  <si>
     <t>dset2.2</t>
   </si>
   <si>
-    <t>(3, 5)</t>
-  </si>
-  <si>
     <t>/g0000</t>
   </si>
   <si>
@@ -761,37 +734,64 @@
     <t>Time,string16,Bid,float32,Ask,float32</t>
   </si>
   <si>
-    <t>(21684,)</t>
-  </si>
-  <si>
     <t>18-09-2011</t>
   </si>
   <si>
-    <t>(2470,)</t>
-  </si>
-  <si>
     <t>19-09-2011</t>
   </si>
   <si>
-    <t>(14711,)</t>
-  </si>
-  <si>
     <t>22-09-2011</t>
   </si>
   <si>
-    <t>(23536,)</t>
-  </si>
-  <si>
     <t>20-09-2011</t>
   </si>
   <si>
-    <t>(16954,)</t>
-  </si>
-  <si>
     <t>23-09-2011</t>
   </si>
   <si>
-    <t>(17969,)</t>
+    <t>{ 21684 }</t>
+  </si>
+  <si>
+    <t>{ 2470 }</t>
+  </si>
+  <si>
+    <t>{ 14711 }</t>
+  </si>
+  <si>
+    <t>{ 23536 }</t>
+  </si>
+  <si>
+    <t>{ 16954 }</t>
+  </si>
+  <si>
+    <t>{ 17969 }</t>
+  </si>
+  <si>
+    <t>{ 5554, 145 }</t>
+  </si>
+  <si>
+    <t>{ 5554 }</t>
+  </si>
+  <si>
+    <t>{ 5554, 1 }</t>
+  </si>
+  <si>
+    <t>{ 145 }</t>
+  </si>
+  <si>
+    <t>{}</t>
+  </si>
+  <si>
+    <t>{ 10, 10 }</t>
+  </si>
+  <si>
+    <t>{ 20 }</t>
+  </si>
+  <si>
+    <t>{ 10 }</t>
+  </si>
+  <si>
+    <t>{ 3, 5 }</t>
   </si>
 </sst>
 </file>
@@ -1180,7 +1180,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1212,7 +1212,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
       <c r="B5" t="str">
         <f>CONCATENATE($B1,"testfiles\cadchftickdata.h5")</f>
@@ -1420,7 +1420,7 @@
         <v>2</v>
       </c>
       <c r="H10" t="s">
-        <v>24</v>
+        <v>249</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -1431,19 +1431,19 @@
         <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D11">
         <v>5</v>
       </c>
       <c r="F11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G11">
         <v>2</v>
       </c>
       <c r="H11" t="s">
-        <v>24</v>
+        <v>249</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1454,19 +1454,19 @@
         <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D12">
         <v>5</v>
       </c>
       <c r="F12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G12">
         <v>1</v>
       </c>
       <c r="H12" t="s">
-        <v>28</v>
+        <v>250</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1477,19 +1477,19 @@
         <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D13">
         <v>5</v>
       </c>
       <c r="F13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G13">
         <v>2</v>
       </c>
       <c r="H13" t="s">
-        <v>24</v>
+        <v>249</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1500,7 +1500,7 @@
         <v>21</v>
       </c>
       <c r="C14" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D14">
         <v>5</v>
@@ -1512,7 +1512,7 @@
         <v>1</v>
       </c>
       <c r="H14" t="s">
-        <v>28</v>
+        <v>250</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1523,7 +1523,7 @@
         <v>21</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D15">
         <v>5</v>
@@ -1535,7 +1535,7 @@
         <v>2</v>
       </c>
       <c r="H15" t="s">
-        <v>24</v>
+        <v>249</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1546,19 +1546,19 @@
         <v>21</v>
       </c>
       <c r="C16" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D16">
         <v>5</v>
       </c>
       <c r="F16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G16">
         <v>2</v>
       </c>
       <c r="H16" t="s">
-        <v>24</v>
+        <v>249</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1569,19 +1569,19 @@
         <v>21</v>
       </c>
       <c r="C17" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D17">
         <v>5</v>
       </c>
       <c r="F17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G17">
         <v>1</v>
       </c>
       <c r="H17" t="s">
-        <v>28</v>
+        <v>250</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1592,19 +1592,19 @@
         <v>21</v>
       </c>
       <c r="C18" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D18">
         <v>5</v>
       </c>
       <c r="F18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G18">
         <v>2</v>
       </c>
       <c r="H18" t="s">
-        <v>24</v>
+        <v>249</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1615,7 +1615,7 @@
         <v>21</v>
       </c>
       <c r="C19" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D19">
         <v>5</v>
@@ -1627,7 +1627,7 @@
         <v>1</v>
       </c>
       <c r="H19" t="s">
-        <v>28</v>
+        <v>250</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1638,7 +1638,7 @@
         <v>21</v>
       </c>
       <c r="C20" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D20">
         <v>5</v>
@@ -1650,7 +1650,7 @@
         <v>2</v>
       </c>
       <c r="H20" t="s">
-        <v>24</v>
+        <v>249</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -1661,19 +1661,19 @@
         <v>21</v>
       </c>
       <c r="C21" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D21">
         <v>5</v>
       </c>
       <c r="F21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G21">
         <v>2</v>
       </c>
       <c r="H21" t="s">
-        <v>24</v>
+        <v>249</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -1684,19 +1684,19 @@
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D22">
         <v>5</v>
       </c>
       <c r="F22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G22">
         <v>1</v>
       </c>
       <c r="H22" t="s">
-        <v>28</v>
+        <v>250</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1707,19 +1707,19 @@
         <v>21</v>
       </c>
       <c r="C23" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D23">
         <v>5</v>
       </c>
       <c r="F23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G23">
         <v>2</v>
       </c>
       <c r="H23" t="s">
-        <v>24</v>
+        <v>249</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -1730,7 +1730,7 @@
         <v>21</v>
       </c>
       <c r="C24" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D24">
         <v>5</v>
@@ -1742,7 +1742,7 @@
         <v>1</v>
       </c>
       <c r="H24" t="s">
-        <v>28</v>
+        <v>250</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -1753,7 +1753,7 @@
         <v>21</v>
       </c>
       <c r="C25" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D25">
         <v>5</v>
@@ -1765,7 +1765,7 @@
         <v>2</v>
       </c>
       <c r="H25" t="s">
-        <v>24</v>
+        <v>249</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -1776,19 +1776,19 @@
         <v>21</v>
       </c>
       <c r="C26" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D26">
         <v>5</v>
       </c>
       <c r="F26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G26">
         <v>2</v>
       </c>
       <c r="H26" t="s">
-        <v>24</v>
+        <v>249</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -1799,19 +1799,19 @@
         <v>21</v>
       </c>
       <c r="C27" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D27">
         <v>5</v>
       </c>
       <c r="F27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G27">
         <v>1</v>
       </c>
       <c r="H27" t="s">
-        <v>28</v>
+        <v>250</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -1822,19 +1822,19 @@
         <v>21</v>
       </c>
       <c r="C28" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D28">
         <v>5</v>
       </c>
       <c r="F28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G28">
         <v>2</v>
       </c>
       <c r="H28" t="s">
-        <v>24</v>
+        <v>249</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -1845,7 +1845,7 @@
         <v>21</v>
       </c>
       <c r="C29" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D29">
         <v>5</v>
@@ -1857,7 +1857,7 @@
         <v>1</v>
       </c>
       <c r="H29" t="s">
-        <v>28</v>
+        <v>250</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -1868,7 +1868,7 @@
         <v>21</v>
       </c>
       <c r="C30" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D30">
         <v>5</v>
@@ -1880,7 +1880,7 @@
         <v>2</v>
       </c>
       <c r="H30" t="s">
-        <v>24</v>
+        <v>249</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -1891,19 +1891,19 @@
         <v>21</v>
       </c>
       <c r="C31" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D31">
         <v>5</v>
       </c>
       <c r="F31" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G31">
         <v>2</v>
       </c>
       <c r="H31" t="s">
-        <v>24</v>
+        <v>249</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -1914,19 +1914,19 @@
         <v>21</v>
       </c>
       <c r="C32" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D32">
         <v>5</v>
       </c>
       <c r="F32" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G32">
         <v>1</v>
       </c>
       <c r="H32" t="s">
-        <v>28</v>
+        <v>250</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -1937,19 +1937,19 @@
         <v>21</v>
       </c>
       <c r="C33" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D33">
         <v>5</v>
       </c>
       <c r="F33" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G33">
         <v>2</v>
       </c>
       <c r="H33" t="s">
-        <v>24</v>
+        <v>249</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -1960,7 +1960,7 @@
         <v>21</v>
       </c>
       <c r="C34" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D34">
         <v>5</v>
@@ -1972,7 +1972,7 @@
         <v>1</v>
       </c>
       <c r="H34" t="s">
-        <v>28</v>
+        <v>250</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -1983,19 +1983,19 @@
         <v>21</v>
       </c>
       <c r="C35" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D35">
         <v>5</v>
       </c>
       <c r="F35" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G35">
         <v>2</v>
       </c>
       <c r="H35" t="s">
-        <v>24</v>
+        <v>249</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -2006,19 +2006,19 @@
         <v>21</v>
       </c>
       <c r="C36" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D36">
         <v>5</v>
       </c>
       <c r="F36" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G36">
         <v>1</v>
       </c>
       <c r="H36" t="s">
-        <v>28</v>
+        <v>250</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -2029,19 +2029,19 @@
         <v>21</v>
       </c>
       <c r="C37" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D37">
         <v>5</v>
       </c>
       <c r="F37" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G37">
         <v>2</v>
       </c>
       <c r="H37" t="s">
-        <v>24</v>
+        <v>249</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -2052,7 +2052,7 @@
         <v>21</v>
       </c>
       <c r="C38" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D38">
         <v>5</v>
@@ -2064,7 +2064,7 @@
         <v>1</v>
       </c>
       <c r="H38" t="s">
-        <v>28</v>
+        <v>250</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -2075,19 +2075,19 @@
         <v>21</v>
       </c>
       <c r="C39" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D39">
         <v>5</v>
       </c>
       <c r="F39" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G39">
         <v>2</v>
       </c>
       <c r="H39" t="s">
-        <v>24</v>
+        <v>249</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -2098,19 +2098,19 @@
         <v>21</v>
       </c>
       <c r="C40" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D40">
         <v>5</v>
       </c>
       <c r="F40" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G40">
         <v>1</v>
       </c>
       <c r="H40" t="s">
-        <v>28</v>
+        <v>250</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -2121,19 +2121,19 @@
         <v>21</v>
       </c>
       <c r="C41" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D41">
         <v>5</v>
       </c>
       <c r="F41" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G41">
         <v>2</v>
       </c>
       <c r="H41" t="s">
-        <v>24</v>
+        <v>249</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -2144,7 +2144,7 @@
         <v>21</v>
       </c>
       <c r="C42" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D42">
         <v>5</v>
@@ -2156,7 +2156,7 @@
         <v>1</v>
       </c>
       <c r="H42" t="s">
-        <v>28</v>
+        <v>250</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -2167,19 +2167,19 @@
         <v>21</v>
       </c>
       <c r="C43" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D43">
         <v>5</v>
       </c>
       <c r="F43" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G43">
         <v>2</v>
       </c>
       <c r="H43" t="s">
-        <v>24</v>
+        <v>249</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -2190,19 +2190,19 @@
         <v>21</v>
       </c>
       <c r="C44" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D44">
         <v>5</v>
       </c>
       <c r="F44" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G44">
         <v>1</v>
       </c>
       <c r="H44" t="s">
-        <v>28</v>
+        <v>250</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -2213,19 +2213,19 @@
         <v>21</v>
       </c>
       <c r="C45" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D45">
         <v>5</v>
       </c>
       <c r="F45" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G45">
         <v>2</v>
       </c>
       <c r="H45" t="s">
-        <v>24</v>
+        <v>249</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -2236,7 +2236,7 @@
         <v>21</v>
       </c>
       <c r="C46" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D46">
         <v>5</v>
@@ -2248,7 +2248,7 @@
         <v>1</v>
       </c>
       <c r="H46" t="s">
-        <v>28</v>
+        <v>250</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -2259,19 +2259,19 @@
         <v>21</v>
       </c>
       <c r="C47" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D47">
         <v>5</v>
       </c>
       <c r="F47" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G47">
         <v>2</v>
       </c>
       <c r="H47" t="s">
-        <v>24</v>
+        <v>249</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -2282,19 +2282,19 @@
         <v>21</v>
       </c>
       <c r="C48" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D48">
         <v>5</v>
       </c>
       <c r="F48" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G48">
         <v>1</v>
       </c>
       <c r="H48" t="s">
-        <v>28</v>
+        <v>250</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
@@ -2305,19 +2305,19 @@
         <v>21</v>
       </c>
       <c r="C49" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D49">
         <v>5</v>
       </c>
       <c r="F49" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G49">
         <v>2</v>
       </c>
       <c r="H49" t="s">
-        <v>24</v>
+        <v>249</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
@@ -2328,7 +2328,7 @@
         <v>21</v>
       </c>
       <c r="C50" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D50">
         <v>5</v>
@@ -2340,7 +2340,7 @@
         <v>1</v>
       </c>
       <c r="H50" t="s">
-        <v>28</v>
+        <v>250</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -2351,19 +2351,19 @@
         <v>21</v>
       </c>
       <c r="C51" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D51">
         <v>5</v>
       </c>
       <c r="F51" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G51">
         <v>2</v>
       </c>
       <c r="H51" t="s">
-        <v>68</v>
+        <v>251</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
@@ -2374,19 +2374,19 @@
         <v>21</v>
       </c>
       <c r="C52" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D52">
         <v>5</v>
       </c>
       <c r="F52" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G52">
         <v>2</v>
       </c>
       <c r="H52" t="s">
-        <v>24</v>
+        <v>249</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
@@ -2397,19 +2397,19 @@
         <v>21</v>
       </c>
       <c r="C53" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D53">
         <v>5</v>
       </c>
       <c r="F53" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G53">
         <v>1</v>
       </c>
       <c r="H53" t="s">
-        <v>28</v>
+        <v>250</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
@@ -2420,19 +2420,19 @@
         <v>21</v>
       </c>
       <c r="C54" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D54">
         <v>5</v>
       </c>
       <c r="F54" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G54">
         <v>2</v>
       </c>
       <c r="H54" t="s">
-        <v>24</v>
+        <v>249</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
@@ -2443,7 +2443,7 @@
         <v>21</v>
       </c>
       <c r="C55" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D55">
         <v>5</v>
@@ -2455,7 +2455,7 @@
         <v>1</v>
       </c>
       <c r="H55" t="s">
-        <v>28</v>
+        <v>250</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
@@ -2466,19 +2466,19 @@
         <v>21</v>
       </c>
       <c r="C56" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D56">
         <v>5</v>
       </c>
       <c r="F56" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G56">
         <v>2</v>
       </c>
       <c r="H56" t="s">
-        <v>24</v>
+        <v>249</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
@@ -2489,19 +2489,19 @@
         <v>21</v>
       </c>
       <c r="C57" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D57">
         <v>5</v>
       </c>
       <c r="F57" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G57">
         <v>1</v>
       </c>
       <c r="H57" t="s">
-        <v>28</v>
+        <v>250</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
@@ -2512,19 +2512,19 @@
         <v>21</v>
       </c>
       <c r="C58" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D58">
         <v>5</v>
       </c>
       <c r="F58" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G58">
         <v>2</v>
       </c>
       <c r="H58" t="s">
-        <v>24</v>
+        <v>249</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
@@ -2535,7 +2535,7 @@
         <v>21</v>
       </c>
       <c r="C59" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D59">
         <v>5</v>
@@ -2547,7 +2547,7 @@
         <v>1</v>
       </c>
       <c r="H59" t="s">
-        <v>28</v>
+        <v>250</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
@@ -2558,19 +2558,19 @@
         <v>21</v>
       </c>
       <c r="C60" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D60">
         <v>5</v>
       </c>
       <c r="F60" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G60">
         <v>2</v>
       </c>
       <c r="H60" t="s">
-        <v>24</v>
+        <v>249</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
@@ -2581,19 +2581,19 @@
         <v>21</v>
       </c>
       <c r="C61" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D61">
         <v>5</v>
       </c>
       <c r="F61" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G61">
         <v>2</v>
       </c>
       <c r="H61" t="s">
-        <v>24</v>
+        <v>249</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
@@ -2604,19 +2604,19 @@
         <v>21</v>
       </c>
       <c r="C62" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D62">
         <v>5</v>
       </c>
       <c r="F62" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G62">
         <v>1</v>
       </c>
       <c r="H62" t="s">
-        <v>28</v>
+        <v>250</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
@@ -2627,19 +2627,19 @@
         <v>21</v>
       </c>
       <c r="C63" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D63">
         <v>5</v>
       </c>
       <c r="F63" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G63">
         <v>2</v>
       </c>
       <c r="H63" t="s">
-        <v>24</v>
+        <v>249</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
@@ -2650,7 +2650,7 @@
         <v>21</v>
       </c>
       <c r="C64" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D64">
         <v>5</v>
@@ -2662,7 +2662,7 @@
         <v>1</v>
       </c>
       <c r="H64" t="s">
-        <v>28</v>
+        <v>250</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
@@ -2673,19 +2673,19 @@
         <v>21</v>
       </c>
       <c r="C65" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D65">
         <v>5</v>
       </c>
       <c r="F65" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G65">
         <v>1</v>
       </c>
       <c r="H65" t="s">
-        <v>28</v>
+        <v>250</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
@@ -2696,19 +2696,19 @@
         <v>21</v>
       </c>
       <c r="C66" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D66">
         <v>5</v>
       </c>
       <c r="F66" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G66">
         <v>2</v>
       </c>
       <c r="H66" t="s">
-        <v>24</v>
+        <v>249</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
@@ -2719,7 +2719,7 @@
         <v>21</v>
       </c>
       <c r="C67" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D67">
         <v>5</v>
@@ -2731,7 +2731,7 @@
         <v>1</v>
       </c>
       <c r="H67" t="s">
-        <v>28</v>
+        <v>250</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
@@ -2742,19 +2742,19 @@
         <v>21</v>
       </c>
       <c r="C68" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D68">
         <v>5</v>
       </c>
       <c r="F68" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G68">
         <v>2</v>
       </c>
       <c r="H68" t="s">
-        <v>24</v>
+        <v>249</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
@@ -2765,19 +2765,19 @@
         <v>21</v>
       </c>
       <c r="C69" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D69">
         <v>5</v>
       </c>
       <c r="F69" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G69">
         <v>1</v>
       </c>
       <c r="H69" t="s">
-        <v>28</v>
+        <v>250</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
@@ -2788,19 +2788,19 @@
         <v>21</v>
       </c>
       <c r="C70" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D70">
         <v>5</v>
       </c>
       <c r="F70" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G70">
         <v>2</v>
       </c>
       <c r="H70" t="s">
-        <v>24</v>
+        <v>249</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
@@ -2811,7 +2811,7 @@
         <v>21</v>
       </c>
       <c r="C71" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D71">
         <v>5</v>
@@ -2823,7 +2823,7 @@
         <v>1</v>
       </c>
       <c r="H71" t="s">
-        <v>28</v>
+        <v>250</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
@@ -2834,19 +2834,19 @@
         <v>21</v>
       </c>
       <c r="C72" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D72">
         <v>5</v>
       </c>
       <c r="F72" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G72">
         <v>2</v>
       </c>
       <c r="H72" t="s">
-        <v>24</v>
+        <v>249</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
@@ -2857,19 +2857,19 @@
         <v>21</v>
       </c>
       <c r="C73" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D73">
         <v>5</v>
       </c>
       <c r="F73" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G73">
         <v>1</v>
       </c>
       <c r="H73" t="s">
-        <v>28</v>
+        <v>250</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
@@ -2880,19 +2880,19 @@
         <v>21</v>
       </c>
       <c r="C74" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D74">
         <v>5</v>
       </c>
       <c r="F74" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G74">
         <v>2</v>
       </c>
       <c r="H74" t="s">
-        <v>24</v>
+        <v>249</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
@@ -2903,7 +2903,7 @@
         <v>21</v>
       </c>
       <c r="C75" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D75">
         <v>5</v>
@@ -2915,7 +2915,7 @@
         <v>1</v>
       </c>
       <c r="H75" t="s">
-        <v>28</v>
+        <v>250</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
@@ -2926,19 +2926,19 @@
         <v>21</v>
       </c>
       <c r="C76" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D76">
         <v>5</v>
       </c>
       <c r="F76" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G76">
         <v>2</v>
       </c>
       <c r="H76" t="s">
-        <v>24</v>
+        <v>249</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
@@ -2949,19 +2949,19 @@
         <v>21</v>
       </c>
       <c r="C77" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D77">
         <v>5</v>
       </c>
       <c r="F77" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G77">
         <v>1</v>
       </c>
       <c r="H77" t="s">
-        <v>28</v>
+        <v>250</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
@@ -2972,19 +2972,19 @@
         <v>21</v>
       </c>
       <c r="C78" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D78">
         <v>5</v>
       </c>
       <c r="F78" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G78">
         <v>2</v>
       </c>
       <c r="H78" t="s">
-        <v>24</v>
+        <v>249</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
@@ -2995,7 +2995,7 @@
         <v>21</v>
       </c>
       <c r="C79" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D79">
         <v>5</v>
@@ -3007,7 +3007,7 @@
         <v>1</v>
       </c>
       <c r="H79" t="s">
-        <v>28</v>
+        <v>250</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
@@ -3018,7 +3018,7 @@
         <v>13</v>
       </c>
       <c r="C80" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D80">
         <v>0</v>
@@ -3035,19 +3035,19 @@
         <v>21</v>
       </c>
       <c r="C81" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D81">
         <v>5</v>
       </c>
       <c r="F81" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G81">
         <v>2</v>
       </c>
       <c r="H81" t="s">
-        <v>24</v>
+        <v>249</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
@@ -3058,19 +3058,19 @@
         <v>21</v>
       </c>
       <c r="C82" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D82">
         <v>5</v>
       </c>
       <c r="F82" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G82">
         <v>1</v>
       </c>
       <c r="H82" t="s">
-        <v>28</v>
+        <v>250</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
@@ -3081,19 +3081,19 @@
         <v>21</v>
       </c>
       <c r="C83" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D83">
         <v>5</v>
       </c>
       <c r="F83" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G83">
         <v>1</v>
       </c>
       <c r="H83" t="s">
-        <v>28</v>
+        <v>250</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
@@ -3104,19 +3104,19 @@
         <v>21</v>
       </c>
       <c r="C84" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D84">
         <v>5</v>
       </c>
       <c r="F84" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G84">
         <v>1</v>
       </c>
       <c r="H84" t="s">
-        <v>28</v>
+        <v>250</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
@@ -3127,7 +3127,7 @@
         <v>21</v>
       </c>
       <c r="C85" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D85">
         <v>5</v>
@@ -3139,7 +3139,7 @@
         <v>1</v>
       </c>
       <c r="H85" t="s">
-        <v>28</v>
+        <v>250</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
@@ -3150,19 +3150,19 @@
         <v>21</v>
       </c>
       <c r="C86" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D86">
         <v>5</v>
       </c>
       <c r="F86" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G86">
         <v>1</v>
       </c>
       <c r="H86" t="s">
-        <v>104</v>
+        <v>252</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
@@ -3173,19 +3173,19 @@
         <v>21</v>
       </c>
       <c r="C87" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D87">
         <v>5</v>
       </c>
       <c r="F87" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="G87">
         <v>1</v>
       </c>
       <c r="H87" t="s">
-        <v>28</v>
+        <v>250</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
@@ -3196,19 +3196,19 @@
         <v>21</v>
       </c>
       <c r="C88" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D88">
         <v>5</v>
       </c>
       <c r="F88" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G88">
         <v>1</v>
       </c>
       <c r="H88" t="s">
-        <v>28</v>
+        <v>250</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
@@ -3219,19 +3219,19 @@
         <v>21</v>
       </c>
       <c r="C89" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D89">
         <v>5</v>
       </c>
       <c r="F89" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G89">
         <v>1</v>
       </c>
       <c r="H89" t="s">
-        <v>28</v>
+        <v>250</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
@@ -3242,19 +3242,19 @@
         <v>21</v>
       </c>
       <c r="C90" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D90">
         <v>5</v>
       </c>
       <c r="F90" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="G90">
         <v>1</v>
       </c>
       <c r="H90" t="s">
-        <v>28</v>
+        <v>250</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
@@ -3265,7 +3265,7 @@
         <v>21</v>
       </c>
       <c r="C91" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D91">
         <v>5</v>
@@ -3277,7 +3277,7 @@
         <v>1</v>
       </c>
       <c r="H91" t="s">
-        <v>28</v>
+        <v>250</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
@@ -3288,19 +3288,19 @@
         <v>21</v>
       </c>
       <c r="C92" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D92">
         <v>5</v>
       </c>
       <c r="F92" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="G92">
         <v>1</v>
       </c>
       <c r="H92" t="s">
-        <v>28</v>
+        <v>250</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
@@ -3311,19 +3311,19 @@
         <v>21</v>
       </c>
       <c r="C93" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D93">
         <v>5</v>
       </c>
       <c r="F93" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G93">
         <v>1</v>
       </c>
       <c r="H93" t="s">
-        <v>28</v>
+        <v>250</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
@@ -3334,19 +3334,19 @@
         <v>21</v>
       </c>
       <c r="C94" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D94">
         <v>5</v>
       </c>
       <c r="F94" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G94">
         <v>1</v>
       </c>
       <c r="H94" t="s">
-        <v>28</v>
+        <v>250</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
@@ -3357,19 +3357,19 @@
         <v>21</v>
       </c>
       <c r="C95" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D95">
         <v>5</v>
       </c>
       <c r="F95" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G95">
         <v>1</v>
       </c>
       <c r="H95" t="s">
-        <v>28</v>
+        <v>250</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
@@ -3380,19 +3380,19 @@
         <v>21</v>
       </c>
       <c r="C96" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D96">
         <v>5</v>
       </c>
       <c r="F96" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G96">
         <v>1</v>
       </c>
       <c r="H96" t="s">
-        <v>28</v>
+        <v>250</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
@@ -3403,19 +3403,19 @@
         <v>21</v>
       </c>
       <c r="C97" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D97">
         <v>5</v>
       </c>
       <c r="F97" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G97">
         <v>1</v>
       </c>
       <c r="H97" t="s">
-        <v>28</v>
+        <v>250</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
@@ -3426,19 +3426,19 @@
         <v>21</v>
       </c>
       <c r="C98" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D98">
         <v>5</v>
       </c>
       <c r="F98" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G98">
         <v>1</v>
       </c>
       <c r="H98" t="s">
-        <v>28</v>
+        <v>250</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
@@ -3449,19 +3449,19 @@
         <v>21</v>
       </c>
       <c r="C99" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D99">
         <v>5</v>
       </c>
       <c r="F99" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="G99">
         <v>1</v>
       </c>
       <c r="H99" t="s">
-        <v>28</v>
+        <v>250</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
@@ -3472,19 +3472,19 @@
         <v>21</v>
       </c>
       <c r="C100" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D100">
         <v>5</v>
       </c>
       <c r="F100" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G100">
         <v>1</v>
       </c>
       <c r="H100" t="s">
-        <v>28</v>
+        <v>250</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
@@ -3495,7 +3495,7 @@
         <v>13</v>
       </c>
       <c r="C101" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="D101">
         <v>1</v>
@@ -3512,19 +3512,19 @@
         <v>21</v>
       </c>
       <c r="C102" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D102">
         <v>0</v>
       </c>
       <c r="F102" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="G102">
         <v>0</v>
       </c>
       <c r="H102" t="s">
-        <v>124</v>
+        <v>253</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
@@ -3535,19 +3535,19 @@
         <v>21</v>
       </c>
       <c r="C103" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="D103">
         <v>0</v>
       </c>
       <c r="F103" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="G103">
         <v>0</v>
       </c>
       <c r="H103" t="s">
-        <v>124</v>
+        <v>253</v>
       </c>
     </row>
   </sheetData>
@@ -3634,7 +3634,7 @@
         <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -3651,7 +3651,7 @@
         <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -3665,22 +3665,22 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="C6" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="D6">
         <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="G6">
         <v>2</v>
       </c>
       <c r="H6" t="s">
-        <v>130</v>
+        <v>254</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -3688,22 +3688,22 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="C7" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
       <c r="F7" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="G7">
         <v>1</v>
       </c>
       <c r="H7" t="s">
-        <v>132</v>
+        <v>255</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -3714,7 +3714,7 @@
         <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -3731,7 +3731,7 @@
         <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -3748,7 +3748,7 @@
         <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -3762,22 +3762,22 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="C11" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="D11">
         <v>0</v>
       </c>
       <c r="F11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G11">
         <v>1</v>
       </c>
       <c r="H11" t="s">
-        <v>137</v>
+        <v>256</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -3785,22 +3785,22 @@
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="C12" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="D12">
         <v>0</v>
       </c>
       <c r="F12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G12">
         <v>2</v>
       </c>
       <c r="H12" t="s">
-        <v>139</v>
+        <v>257</v>
       </c>
     </row>
   </sheetData>
@@ -3812,7 +3812,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I103"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3884,7 +3886,7 @@
         <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -3901,7 +3903,7 @@
         <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -3918,7 +3920,7 @@
         <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -3935,7 +3937,7 @@
         <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -3952,7 +3954,7 @@
         <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -3969,7 +3971,7 @@
         <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -3986,7 +3988,7 @@
         <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -4003,7 +4005,7 @@
         <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -4020,7 +4022,7 @@
         <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -4037,7 +4039,7 @@
         <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -4054,7 +4056,7 @@
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -4071,7 +4073,7 @@
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -4088,7 +4090,7 @@
         <v>13</v>
       </c>
       <c r="C16" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -4105,7 +4107,7 @@
         <v>13</v>
       </c>
       <c r="C17" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -4122,7 +4124,7 @@
         <v>13</v>
       </c>
       <c r="C18" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -4139,7 +4141,7 @@
         <v>13</v>
       </c>
       <c r="C19" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -4156,7 +4158,7 @@
         <v>13</v>
       </c>
       <c r="C20" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -4173,7 +4175,7 @@
         <v>13</v>
       </c>
       <c r="C21" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -4190,7 +4192,7 @@
         <v>13</v>
       </c>
       <c r="C22" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -4207,7 +4209,7 @@
         <v>13</v>
       </c>
       <c r="C23" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -4224,7 +4226,7 @@
         <v>13</v>
       </c>
       <c r="C24" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="D24">
         <v>0</v>
@@ -4241,7 +4243,7 @@
         <v>13</v>
       </c>
       <c r="C25" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -4258,7 +4260,7 @@
         <v>13</v>
       </c>
       <c r="C26" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="D26">
         <v>0</v>
@@ -4275,7 +4277,7 @@
         <v>13</v>
       </c>
       <c r="C27" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="D27">
         <v>0</v>
@@ -4292,7 +4294,7 @@
         <v>13</v>
       </c>
       <c r="C28" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="D28">
         <v>0</v>
@@ -4309,7 +4311,7 @@
         <v>13</v>
       </c>
       <c r="C29" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="D29">
         <v>0</v>
@@ -4326,7 +4328,7 @@
         <v>13</v>
       </c>
       <c r="C30" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="D30">
         <v>0</v>
@@ -4343,7 +4345,7 @@
         <v>13</v>
       </c>
       <c r="C31" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="D31">
         <v>0</v>
@@ -4360,7 +4362,7 @@
         <v>13</v>
       </c>
       <c r="C32" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="D32">
         <v>0</v>
@@ -4377,7 +4379,7 @@
         <v>13</v>
       </c>
       <c r="C33" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="D33">
         <v>0</v>
@@ -4394,7 +4396,7 @@
         <v>13</v>
       </c>
       <c r="C34" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="D34">
         <v>0</v>
@@ -4411,7 +4413,7 @@
         <v>13</v>
       </c>
       <c r="C35" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="D35">
         <v>0</v>
@@ -4428,7 +4430,7 @@
         <v>13</v>
       </c>
       <c r="C36" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="D36">
         <v>0</v>
@@ -4445,7 +4447,7 @@
         <v>13</v>
       </c>
       <c r="C37" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="D37">
         <v>0</v>
@@ -4462,7 +4464,7 @@
         <v>13</v>
       </c>
       <c r="C38" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="D38">
         <v>0</v>
@@ -4479,7 +4481,7 @@
         <v>13</v>
       </c>
       <c r="C39" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="D39">
         <v>0</v>
@@ -4496,7 +4498,7 @@
         <v>13</v>
       </c>
       <c r="C40" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="D40">
         <v>0</v>
@@ -4513,7 +4515,7 @@
         <v>13</v>
       </c>
       <c r="C41" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="D41">
         <v>0</v>
@@ -4530,7 +4532,7 @@
         <v>13</v>
       </c>
       <c r="C42" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="D42">
         <v>0</v>
@@ -4547,7 +4549,7 @@
         <v>13</v>
       </c>
       <c r="C43" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="D43">
         <v>0</v>
@@ -4564,7 +4566,7 @@
         <v>13</v>
       </c>
       <c r="C44" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="D44">
         <v>0</v>
@@ -4581,7 +4583,7 @@
         <v>13</v>
       </c>
       <c r="C45" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="D45">
         <v>0</v>
@@ -4598,7 +4600,7 @@
         <v>13</v>
       </c>
       <c r="C46" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="D46">
         <v>0</v>
@@ -4615,7 +4617,7 @@
         <v>13</v>
       </c>
       <c r="C47" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="D47">
         <v>0</v>
@@ -4632,7 +4634,7 @@
         <v>13</v>
       </c>
       <c r="C48" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="D48">
         <v>0</v>
@@ -4649,7 +4651,7 @@
         <v>13</v>
       </c>
       <c r="C49" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="D49">
         <v>0</v>
@@ -4666,7 +4668,7 @@
         <v>13</v>
       </c>
       <c r="C50" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="D50">
         <v>0</v>
@@ -4683,7 +4685,7 @@
         <v>13</v>
       </c>
       <c r="C51" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="D51">
         <v>0</v>
@@ -4700,7 +4702,7 @@
         <v>13</v>
       </c>
       <c r="C52" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="D52">
         <v>0</v>
@@ -4717,7 +4719,7 @@
         <v>13</v>
       </c>
       <c r="C53" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="D53">
         <v>0</v>
@@ -4734,7 +4736,7 @@
         <v>13</v>
       </c>
       <c r="C54" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="D54">
         <v>0</v>
@@ -4751,7 +4753,7 @@
         <v>13</v>
       </c>
       <c r="C55" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="D55">
         <v>0</v>
@@ -4768,7 +4770,7 @@
         <v>13</v>
       </c>
       <c r="C56" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="D56">
         <v>0</v>
@@ -4785,7 +4787,7 @@
         <v>13</v>
       </c>
       <c r="C57" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="D57">
         <v>0</v>
@@ -4802,7 +4804,7 @@
         <v>13</v>
       </c>
       <c r="C58" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="D58">
         <v>0</v>
@@ -4819,7 +4821,7 @@
         <v>13</v>
       </c>
       <c r="C59" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="D59">
         <v>0</v>
@@ -4836,7 +4838,7 @@
         <v>13</v>
       </c>
       <c r="C60" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="D60">
         <v>0</v>
@@ -4853,7 +4855,7 @@
         <v>13</v>
       </c>
       <c r="C61" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="D61">
         <v>0</v>
@@ -4870,7 +4872,7 @@
         <v>13</v>
       </c>
       <c r="C62" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="D62">
         <v>0</v>
@@ -4887,7 +4889,7 @@
         <v>13</v>
       </c>
       <c r="C63" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="D63">
         <v>0</v>
@@ -4904,7 +4906,7 @@
         <v>13</v>
       </c>
       <c r="C64" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="D64">
         <v>0</v>
@@ -4921,7 +4923,7 @@
         <v>13</v>
       </c>
       <c r="C65" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="D65">
         <v>0</v>
@@ -4938,7 +4940,7 @@
         <v>13</v>
       </c>
       <c r="C66" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="D66">
         <v>0</v>
@@ -4955,7 +4957,7 @@
         <v>13</v>
       </c>
       <c r="C67" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="D67">
         <v>0</v>
@@ -4972,7 +4974,7 @@
         <v>13</v>
       </c>
       <c r="C68" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="D68">
         <v>0</v>
@@ -4989,7 +4991,7 @@
         <v>13</v>
       </c>
       <c r="C69" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="D69">
         <v>0</v>
@@ -5006,7 +5008,7 @@
         <v>13</v>
       </c>
       <c r="C70" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="D70">
         <v>0</v>
@@ -5023,7 +5025,7 @@
         <v>13</v>
       </c>
       <c r="C71" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="D71">
         <v>0</v>
@@ -5040,7 +5042,7 @@
         <v>13</v>
       </c>
       <c r="C72" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="D72">
         <v>0</v>
@@ -5057,7 +5059,7 @@
         <v>13</v>
       </c>
       <c r="C73" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="D73">
         <v>0</v>
@@ -5074,7 +5076,7 @@
         <v>13</v>
       </c>
       <c r="C74" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="D74">
         <v>0</v>
@@ -5091,7 +5093,7 @@
         <v>13</v>
       </c>
       <c r="C75" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="D75">
         <v>0</v>
@@ -5108,7 +5110,7 @@
         <v>13</v>
       </c>
       <c r="C76" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="D76">
         <v>0</v>
@@ -5125,7 +5127,7 @@
         <v>13</v>
       </c>
       <c r="C77" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="D77">
         <v>0</v>
@@ -5142,7 +5144,7 @@
         <v>13</v>
       </c>
       <c r="C78" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="D78">
         <v>0</v>
@@ -5159,7 +5161,7 @@
         <v>13</v>
       </c>
       <c r="C79" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="D79">
         <v>0</v>
@@ -5176,7 +5178,7 @@
         <v>13</v>
       </c>
       <c r="C80" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="D80">
         <v>0</v>
@@ -5193,7 +5195,7 @@
         <v>13</v>
       </c>
       <c r="C81" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="D81">
         <v>0</v>
@@ -5210,7 +5212,7 @@
         <v>13</v>
       </c>
       <c r="C82" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="D82">
         <v>0</v>
@@ -5227,7 +5229,7 @@
         <v>13</v>
       </c>
       <c r="C83" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="D83">
         <v>0</v>
@@ -5244,7 +5246,7 @@
         <v>13</v>
       </c>
       <c r="C84" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="D84">
         <v>0</v>
@@ -5261,7 +5263,7 @@
         <v>13</v>
       </c>
       <c r="C85" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="D85">
         <v>0</v>
@@ -5278,7 +5280,7 @@
         <v>13</v>
       </c>
       <c r="C86" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="D86">
         <v>0</v>
@@ -5295,7 +5297,7 @@
         <v>13</v>
       </c>
       <c r="C87" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="D87">
         <v>0</v>
@@ -5312,7 +5314,7 @@
         <v>13</v>
       </c>
       <c r="C88" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="D88">
         <v>0</v>
@@ -5329,7 +5331,7 @@
         <v>13</v>
       </c>
       <c r="C89" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="D89">
         <v>0</v>
@@ -5346,7 +5348,7 @@
         <v>13</v>
       </c>
       <c r="C90" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="D90">
         <v>0</v>
@@ -5363,7 +5365,7 @@
         <v>13</v>
       </c>
       <c r="C91" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="D91">
         <v>0</v>
@@ -5380,7 +5382,7 @@
         <v>13</v>
       </c>
       <c r="C92" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="D92">
         <v>0</v>
@@ -5397,7 +5399,7 @@
         <v>13</v>
       </c>
       <c r="C93" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="D93">
         <v>0</v>
@@ -5414,7 +5416,7 @@
         <v>13</v>
       </c>
       <c r="C94" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="D94">
         <v>0</v>
@@ -5431,7 +5433,7 @@
         <v>13</v>
       </c>
       <c r="C95" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="D95">
         <v>0</v>
@@ -5448,7 +5450,7 @@
         <v>13</v>
       </c>
       <c r="C96" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="D96">
         <v>0</v>
@@ -5465,7 +5467,7 @@
         <v>13</v>
       </c>
       <c r="C97" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="D97">
         <v>0</v>
@@ -5482,7 +5484,7 @@
         <v>13</v>
       </c>
       <c r="C98" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="D98">
         <v>0</v>
@@ -5499,7 +5501,7 @@
         <v>13</v>
       </c>
       <c r="C99" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="D99">
         <v>0</v>
@@ -5516,7 +5518,7 @@
         <v>13</v>
       </c>
       <c r="C100" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="D100">
         <v>0</v>
@@ -5533,7 +5535,7 @@
         <v>13</v>
       </c>
       <c r="C101" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="D101">
         <v>0</v>
@@ -5550,7 +5552,7 @@
         <v>13</v>
       </c>
       <c r="C102" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="D102">
         <v>0</v>
@@ -5567,7 +5569,7 @@
         <v>13</v>
       </c>
       <c r="C103" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="D103">
         <v>0</v>
@@ -5585,7 +5587,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5649,22 +5653,22 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="C4" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
       <c r="G4">
         <v>1</v>
       </c>
       <c r="H4" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -5672,22 +5676,22 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
+        <v>235</v>
+      </c>
+      <c r="C5" t="s">
+        <v>238</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="F5" t="s">
+        <v>237</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5" t="s">
         <v>244</v>
-      </c>
-      <c r="C5" t="s">
-        <v>248</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="F5" t="s">
-        <v>246</v>
-      </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-      <c r="H5" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -5695,22 +5699,22 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="C6" t="s">
-        <v>250</v>
+        <v>239</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
       <c r="G6">
         <v>1</v>
       </c>
       <c r="H6" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -5718,22 +5722,22 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="C7" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
       <c r="F7" t="s">
+        <v>237</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7" t="s">
         <v>246</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-      <c r="H7" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -5741,22 +5745,22 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="C8" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="D8">
         <v>0</v>
       </c>
       <c r="F8" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
       <c r="G8">
         <v>1</v>
       </c>
       <c r="H8" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -5764,25 +5768,26 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="C9" t="s">
-        <v>256</v>
+        <v>242</v>
       </c>
       <c r="D9">
         <v>0</v>
       </c>
       <c r="F9" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
       <c r="G9">
         <v>1</v>
       </c>
       <c r="H9" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>